<commit_message>
Addition of extra data samples
</commit_message>
<xml_diff>
--- a/DataFiles/2022 Students Schedule - Main.xlsx
+++ b/DataFiles/2022 Students Schedule - Main.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView windowWidth="25600" windowHeight="11940"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$A:$A,Sheet1!$1:$3</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -750,14 +750,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -765,49 +770,200 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FFffffff"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -816,43 +972,228 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92d050"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdae3f3"/>
+        <fgColor rgb="FFDAE3F3"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf8cbad"/>
+        <fgColor rgb="FFF8CBAD"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfff2cc"/>
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFbfbfbf"/>
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFafabab"/>
+        <fgColor rgb="FFAFABAB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -877,16 +1218,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -903,87 +1244,366 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="6" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -994,10 +1614,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1035,71 +1655,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1127,7 +1747,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1150,11 +1770,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1163,13 +1783,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1179,7 +1799,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1188,7 +1808,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1197,7 +1817,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1205,10 +1825,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1268,786 +1888,712 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:BX18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A4" ySplit="3" xSplit="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" style="21" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="62" max="62" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="63" max="63" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="64" max="64" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="65" max="65" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="66" max="66" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="67" max="67" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="68" max="68" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="69" max="69" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="70" max="70" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="71" max="71" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="72" max="72" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="73" max="73" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="74" max="74" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="75" max="75" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="76" max="76" style="22" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.859375" style="1" customWidth="1"/>
+    <col min="2" max="76" width="18.2890625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2">
+    <row r="1" ht="17.25" customHeight="1" spans="2:76">
+      <c r="B1" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="3">
         <v>7</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="3">
         <v>8</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="3">
         <v>9</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="3">
         <v>10</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="3">
         <v>11</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="3">
         <v>12</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="3">
         <v>13</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="3">
         <v>14</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="3">
         <v>15</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="3">
         <v>16</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="3">
         <v>17</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="3">
         <v>18</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="3">
         <v>19</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="3">
         <v>20</v>
       </c>
-      <c r="V1" s="2">
+      <c r="V1" s="3">
         <v>21</v>
       </c>
-      <c r="W1" s="2">
+      <c r="W1" s="3">
         <v>22</v>
       </c>
-      <c r="X1" s="2">
+      <c r="X1" s="3">
         <v>23</v>
       </c>
-      <c r="Y1" s="2">
+      <c r="Y1" s="3">
         <v>24</v>
       </c>
-      <c r="Z1" s="2">
+      <c r="Z1" s="3">
         <v>25</v>
       </c>
-      <c r="AA1" s="2">
+      <c r="AA1" s="3">
         <v>26</v>
       </c>
-      <c r="AB1" s="2">
+      <c r="AB1" s="3">
         <v>27</v>
       </c>
-      <c r="AC1" s="2">
+      <c r="AC1" s="3">
         <v>28</v>
       </c>
-      <c r="AD1" s="2">
+      <c r="AD1" s="3">
         <v>29</v>
       </c>
-      <c r="AE1" s="2">
+      <c r="AE1" s="3">
         <v>30</v>
       </c>
-      <c r="AF1" s="2">
+      <c r="AF1" s="3">
         <v>31</v>
       </c>
-      <c r="AG1" s="2">
+      <c r="AG1" s="3">
         <v>32</v>
       </c>
-      <c r="AH1" s="2">
+      <c r="AH1" s="3">
         <v>33</v>
       </c>
-      <c r="AI1" s="2">
+      <c r="AI1" s="3">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2">
+      <c r="AJ1" s="3">
         <v>35</v>
       </c>
-      <c r="AK1" s="2">
+      <c r="AK1" s="3">
         <v>36</v>
       </c>
-      <c r="AL1" s="2">
+      <c r="AL1" s="3">
         <v>37</v>
       </c>
-      <c r="AM1" s="2">
+      <c r="AM1" s="3">
         <v>38</v>
       </c>
-      <c r="AN1" s="2">
+      <c r="AN1" s="3">
         <v>39</v>
       </c>
-      <c r="AO1" s="2">
+      <c r="AO1" s="3">
         <v>40</v>
       </c>
-      <c r="AP1" s="2">
+      <c r="AP1" s="3">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2">
+      <c r="AQ1" s="3">
         <v>42</v>
       </c>
-      <c r="AR1" s="2">
+      <c r="AR1" s="3">
         <v>43</v>
       </c>
-      <c r="AS1" s="2">
+      <c r="AS1" s="3">
         <v>44</v>
       </c>
-      <c r="AT1" s="2">
+      <c r="AT1" s="3">
         <v>45</v>
       </c>
-      <c r="AU1" s="2">
+      <c r="AU1" s="3">
         <v>46</v>
       </c>
-      <c r="AV1" s="2">
+      <c r="AV1" s="3">
         <v>47</v>
       </c>
-      <c r="AW1" s="2">
+      <c r="AW1" s="3">
         <v>48</v>
       </c>
-      <c r="AX1" s="2">
+      <c r="AX1" s="3">
         <v>49</v>
       </c>
-      <c r="AY1" s="2">
+      <c r="AY1" s="3">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2">
+      <c r="AZ1" s="3">
         <v>51</v>
       </c>
-      <c r="BA1" s="2">
+      <c r="BA1" s="3">
         <v>52</v>
       </c>
-      <c r="BB1" s="2">
+      <c r="BB1" s="3">
         <v>53</v>
       </c>
-      <c r="BC1" s="2">
+      <c r="BC1" s="3">
         <v>54</v>
       </c>
-      <c r="BD1" s="2">
+      <c r="BD1" s="3">
         <v>55</v>
       </c>
-      <c r="BE1" s="2">
+      <c r="BE1" s="3">
         <v>56</v>
       </c>
-      <c r="BF1" s="2">
+      <c r="BF1" s="3">
         <v>57</v>
       </c>
-      <c r="BG1" s="2">
+      <c r="BG1" s="3">
         <v>58</v>
       </c>
-      <c r="BH1" s="2">
+      <c r="BH1" s="3">
         <v>59</v>
       </c>
-      <c r="BI1" s="2">
+      <c r="BI1" s="3">
         <v>60</v>
       </c>
-      <c r="BJ1" s="2">
+      <c r="BJ1" s="3">
         <v>61</v>
       </c>
-      <c r="BK1" s="2">
+      <c r="BK1" s="3">
         <v>62</v>
       </c>
-      <c r="BL1" s="2">
+      <c r="BL1" s="3">
         <v>63</v>
       </c>
-      <c r="BM1" s="2">
+      <c r="BM1" s="3">
         <v>64</v>
       </c>
-      <c r="BN1" s="2">
+      <c r="BN1" s="3">
         <v>65</v>
       </c>
-      <c r="BO1" s="2">
+      <c r="BO1" s="3">
         <v>66</v>
       </c>
-      <c r="BP1" s="2">
+      <c r="BP1" s="3">
         <v>67</v>
       </c>
-      <c r="BQ1" s="2">
+      <c r="BQ1" s="3">
         <v>68</v>
       </c>
-      <c r="BR1" s="2">
+      <c r="BR1" s="3">
         <v>69</v>
       </c>
-      <c r="BS1" s="2">
+      <c r="BS1" s="3">
         <v>70</v>
       </c>
-      <c r="BT1" s="2">
+      <c r="BT1" s="3">
         <v>71</v>
       </c>
-      <c r="BU1" s="2">
+      <c r="BU1" s="3">
         <v>72</v>
       </c>
-      <c r="BV1" s="2">
+      <c r="BV1" s="3">
         <v>73</v>
       </c>
-      <c r="BW1" s="2">
+      <c r="BW1" s="3">
         <v>74</v>
       </c>
-      <c r="BX1" s="2">
+      <c r="BX1" s="3">
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+    <row r="2" ht="17.25" customHeight="1" spans="1:76">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AH2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AI2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AL2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AM2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AN2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AO2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AP2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AS2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AT2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AU2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AV2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AW2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AX2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AY2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="AZ2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BA2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BB2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BC2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BD2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BE2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BF2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BG2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="BH2" s="4" t="s">
+      <c r="BH2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BI2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BJ2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BK2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BL2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BM2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="BN2" s="4" t="s">
+      <c r="BN2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="BO2" s="4" t="s">
+      <c r="BO2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="BP2" s="4" t="s">
+      <c r="BP2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="BQ2" s="4" t="s">
+      <c r="BQ2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="BR2" s="4" t="s">
+      <c r="BR2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="BS2" s="4" t="s">
+      <c r="BS2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="BT2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BU2" s="4" t="s">
+      <c r="BU2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BV2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BW2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="BX2" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
+    <row r="3" ht="17.25" customHeight="1" spans="1:76">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="U3" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Y3" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="Z3" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AA3" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AB3" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AC3" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AD3" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AE3" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AF3" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AG3" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AH3" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AI3" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="AJ3" s="6" t="s">
+      <c r="AJ3" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="AK3" s="6" t="s">
+      <c r="AK3" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="AL3" s="6" t="s">
+      <c r="AL3" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="AM3" s="6" t="s">
+      <c r="AM3" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="AN3" s="6" t="s">
+      <c r="AN3" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="AO3" s="6" t="s">
+      <c r="AO3" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="AP3" s="6" t="s">
+      <c r="AP3" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="AQ3" s="6" t="s">
+      <c r="AQ3" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="AR3" s="6" t="s">
+      <c r="AR3" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="AS3" s="6" t="s">
+      <c r="AS3" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="AT3" s="6" t="s">
+      <c r="AT3" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="AU3" s="6" t="s">
+      <c r="AU3" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="AV3" s="4" t="s">
+      <c r="AV3" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="AW3" s="4" t="s">
+      <c r="AW3" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="AX3" s="4" t="s">
+      <c r="AX3" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AY3" s="4" t="s">
+      <c r="AY3" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="AZ3" s="4" t="s">
+      <c r="AZ3" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="BA3" s="4" t="s">
+      <c r="BA3" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="BB3" s="4" t="s">
+      <c r="BB3" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="BC3" s="4" t="s">
+      <c r="BC3" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="BD3" s="4" t="s">
+      <c r="BD3" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="BE3" s="4" t="s">
+      <c r="BE3" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="BF3" s="4" t="s">
+      <c r="BF3" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="BG3" s="4" t="s">
+      <c r="BG3" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="BH3" s="4" t="s">
+      <c r="BH3" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="BI3" s="4" t="s">
+      <c r="BI3" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="BJ3" s="4" t="s">
+      <c r="BJ3" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="BK3" s="4" t="s">
+      <c r="BK3" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="BL3" s="4" t="s">
+      <c r="BL3" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="BM3" s="4" t="s">
+      <c r="BM3" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="BN3" s="4" t="s">
+      <c r="BN3" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="BO3" s="4" t="s">
+      <c r="BO3" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="BP3" s="4" t="s">
+      <c r="BP3" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="BQ3" s="4" t="s">
+      <c r="BQ3" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="BR3" s="4" t="s">
+      <c r="BR3" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="BS3" s="4" t="s">
+      <c r="BS3" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="BT3" s="4" t="s">
+      <c r="BT3" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="BU3" s="4" t="s">
+      <c r="BU3" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="BV3" s="4" t="s">
+      <c r="BV3" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="BW3" s="4" t="s">
+      <c r="BW3" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="BX3" s="4" t="s">
+      <c r="BX3" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="46.5">
+    <row r="4" ht="46.5" customHeight="1" spans="1:76">
       <c r="A4" s="7" t="s">
         <v>150</v>
       </c>
@@ -2081,7 +2627,7 @@
       <c r="K4" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="10" t="s">
         <v>161</v>
       </c>
       <c r="M4" s="8" t="s">
@@ -2105,8 +2651,8 @@
       <c r="S4" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="T4" s="10"/>
-      <c r="U4" s="9" t="s">
+      <c r="T4" s="18"/>
+      <c r="U4" s="10" t="s">
         <v>169</v>
       </c>
       <c r="V4" s="8" t="s">
@@ -2130,14 +2676,14 @@
       <c r="AB4" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="AC4" s="9" t="s">
+      <c r="AC4" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="AD4" s="10"/>
+      <c r="AD4" s="18"/>
       <c r="AE4" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="AF4" s="9" t="s">
+      <c r="AF4" s="10" t="s">
         <v>178</v>
       </c>
       <c r="AG4" s="8" t="s">
@@ -2155,7 +2701,7 @@
       <c r="AK4" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="AL4" s="9" t="s">
+      <c r="AL4" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AM4" s="8" t="s">
@@ -2200,7 +2746,7 @@
       <c r="AZ4" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="BA4" s="10"/>
+      <c r="BA4" s="18"/>
       <c r="BB4" s="8" t="s">
         <v>198</v>
       </c>
@@ -2216,7 +2762,7 @@
       <c r="BF4" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="BG4" s="9" t="s">
+      <c r="BG4" s="10" t="s">
         <v>178</v>
       </c>
       <c r="BH4" s="8" t="s">
@@ -2231,7 +2777,7 @@
       <c r="BK4" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="BL4" s="9" t="s">
+      <c r="BL4" s="10" t="s">
         <v>161</v>
       </c>
       <c r="BM4" s="8" t="s">
@@ -2271,8 +2817,8 @@
         <v>218</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="41.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" ht="41.25" customHeight="1" spans="1:76">
+      <c r="A5" s="9" t="s">
         <v>219</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -2317,7 +2863,7 @@
       <c r="O5" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="10" t="s">
         <v>178</v>
       </c>
       <c r="Q5" s="8" t="s">
@@ -2329,7 +2875,7 @@
       <c r="S5" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="T5" s="10"/>
+      <c r="T5" s="18"/>
       <c r="U5" s="8" t="s">
         <v>181</v>
       </c>
@@ -2354,7 +2900,7 @@
       <c r="AB5" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AC5" s="10" t="s">
         <v>178</v>
       </c>
       <c r="AD5" s="8" t="s">
@@ -2378,7 +2924,7 @@
       <c r="AJ5" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="AK5" s="9" t="s">
+      <c r="AK5" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AL5" s="8" t="s">
@@ -2387,7 +2933,7 @@
       <c r="AM5" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="AN5" s="9" t="s">
+      <c r="AN5" s="10" t="s">
         <v>161</v>
       </c>
       <c r="AO5" s="8" t="s">
@@ -2420,7 +2966,7 @@
       <c r="AX5" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="AY5" s="9" t="s">
+      <c r="AY5" s="10" t="s">
         <v>161</v>
       </c>
       <c r="AZ5" s="8" t="s">
@@ -2480,7 +3026,7 @@
       <c r="BR5" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="BS5" s="9" t="s">
+      <c r="BS5" s="10" t="s">
         <v>172</v>
       </c>
       <c r="BT5" s="8" t="s">
@@ -2489,7 +3035,7 @@
       <c r="BU5" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="BV5" s="12"/>
+      <c r="BV5" s="17"/>
       <c r="BW5" s="8" t="s">
         <v>207</v>
       </c>
@@ -2497,14 +3043,14 @@
         <v>186</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="41.25">
+    <row r="6" ht="41.25" customHeight="1" spans="1:76">
       <c r="A6" s="7" t="s">
         <v>224</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>161</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -2531,7 +3077,7 @@
       <c r="K6" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="10" t="s">
         <v>178</v>
       </c>
       <c r="M6" s="8" t="s">
@@ -2552,10 +3098,10 @@
       <c r="R6" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="S6" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="T6" s="10"/>
+      <c r="T6" s="18"/>
       <c r="U6" s="8" t="s">
         <v>202</v>
       </c>
@@ -2619,7 +3165,7 @@
       <c r="AO6" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="AP6" s="12"/>
+      <c r="AP6" s="17"/>
       <c r="AQ6" s="8" t="s">
         <v>205</v>
       </c>
@@ -2644,7 +3190,7 @@
       <c r="AX6" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="AY6" s="12"/>
+      <c r="AY6" s="17"/>
       <c r="AZ6" s="13"/>
       <c r="BA6" s="8" t="s">
         <v>186</v>
@@ -2664,7 +3210,7 @@
       <c r="BF6" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="BG6" s="9" t="s">
+      <c r="BG6" s="10" t="s">
         <v>161</v>
       </c>
       <c r="BH6" s="8" t="s">
@@ -2676,7 +3222,7 @@
       <c r="BJ6" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="BK6" s="9" t="s">
+      <c r="BK6" s="10" t="s">
         <v>172</v>
       </c>
       <c r="BL6" s="8" t="s">
@@ -2694,7 +3240,7 @@
       <c r="BP6" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="BQ6" s="9" t="s">
+      <c r="BQ6" s="10" t="s">
         <v>172</v>
       </c>
       <c r="BR6" s="8" t="s">
@@ -2719,14 +3265,14 @@
         <v>169</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="41.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" ht="41.25" customHeight="1" spans="1:76">
+      <c r="A7" s="9" t="s">
         <v>227</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>172</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -2766,7 +3312,7 @@
       <c r="P7" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="10" t="s">
         <v>161</v>
       </c>
       <c r="R7" s="8" t="s">
@@ -2775,7 +3321,7 @@
       <c r="S7" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="T7" s="10"/>
+      <c r="T7" s="18"/>
       <c r="U7" s="8" t="s">
         <v>191</v>
       </c>
@@ -2803,7 +3349,7 @@
       <c r="AC7" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="AD7" s="10"/>
+      <c r="AD7" s="18"/>
       <c r="AE7" s="8" t="s">
         <v>220</v>
       </c>
@@ -2822,7 +3368,7 @@
       <c r="AJ7" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="AK7" s="9" t="s">
+      <c r="AK7" s="10" t="s">
         <v>178</v>
       </c>
       <c r="AL7" s="8" t="s">
@@ -2873,7 +3419,7 @@
       <c r="BA7" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="BB7" s="9" t="s">
+      <c r="BB7" s="10" t="s">
         <v>172</v>
       </c>
       <c r="BC7" s="8" t="s">
@@ -2891,7 +3437,7 @@
       <c r="BG7" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="BH7" s="9" t="s">
+      <c r="BH7" s="10" t="s">
         <v>178</v>
       </c>
       <c r="BI7" s="8" t="s">
@@ -2924,7 +3470,7 @@
       <c r="BR7" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="BS7" s="9" t="s">
+      <c r="BS7" s="10" t="s">
         <v>161</v>
       </c>
       <c r="BT7" s="8" t="s">
@@ -2943,7 +3489,7 @@
         <v>170</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="41.25">
+    <row r="8" ht="41.25" customHeight="1" spans="1:76">
       <c r="A8" s="7" t="s">
         <v>228</v>
       </c>
@@ -2980,7 +3526,7 @@
       <c r="L8" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="10" t="s">
         <v>178</v>
       </c>
       <c r="N8" s="8" t="s">
@@ -3001,7 +3547,7 @@
       <c r="S8" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="T8" s="10"/>
+      <c r="T8" s="18"/>
       <c r="U8" s="8" t="s">
         <v>152</v>
       </c>
@@ -3017,7 +3563,7 @@
       <c r="Y8" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="Z8" s="12"/>
+      <c r="Z8" s="17"/>
       <c r="AA8" s="8" t="s">
         <v>174</v>
       </c>
@@ -3027,14 +3573,14 @@
       <c r="AC8" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="AD8" s="10"/>
+      <c r="AD8" s="18"/>
       <c r="AE8" s="8" t="s">
         <v>193</v>
       </c>
       <c r="AF8" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="AG8" s="9" t="s">
+      <c r="AG8" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AH8" s="8" t="s">
@@ -3052,13 +3598,13 @@
       <c r="AL8" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="AM8" s="9" t="s">
+      <c r="AM8" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AN8" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="AO8" s="12"/>
+      <c r="AO8" s="17"/>
       <c r="AP8" s="8" t="s">
         <v>167</v>
       </c>
@@ -3080,7 +3626,7 @@
       <c r="AV8" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="AW8" s="12"/>
+      <c r="AW8" s="17"/>
       <c r="AX8" s="8" t="s">
         <v>201</v>
       </c>
@@ -3153,18 +3699,18 @@
       <c r="BU8" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="BV8" s="9" t="s">
+      <c r="BV8" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="BW8" s="9" t="s">
+      <c r="BW8" s="10" t="s">
         <v>178</v>
       </c>
       <c r="BX8" s="8" t="s">
         <v>211</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="42">
-      <c r="A9" s="11" t="s">
+    <row r="9" ht="42" customHeight="1" spans="1:76">
+      <c r="A9" s="9" t="s">
         <v>229</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -3188,7 +3734,7 @@
       <c r="H9" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="10" t="s">
         <v>172</v>
       </c>
       <c r="J9" s="8" t="s">
@@ -3212,7 +3758,7 @@
       <c r="P9" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="10" t="s">
         <v>178</v>
       </c>
       <c r="R9" s="8" t="s">
@@ -3221,11 +3767,11 @@
       <c r="S9" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="T9" s="10"/>
+      <c r="T9" s="18"/>
       <c r="U9" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="V9" s="9" t="s">
+      <c r="V9" s="10" t="s">
         <v>172</v>
       </c>
       <c r="W9" s="8" t="s">
@@ -3261,16 +3807,16 @@
       <c r="AG9" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="AH9" s="9" t="s">
+      <c r="AH9" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="AI9" s="9" t="s">
+      <c r="AI9" s="10" t="s">
         <v>161</v>
       </c>
       <c r="AJ9" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="AK9" s="9" t="s">
+      <c r="AK9" s="10" t="s">
         <v>161</v>
       </c>
       <c r="AL9" s="8" t="s">
@@ -3336,7 +3882,7 @@
       <c r="BF9" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="BG9" s="12"/>
+      <c r="BG9" s="17"/>
       <c r="BH9" s="8" t="s">
         <v>180</v>
       </c>
@@ -3389,87 +3935,87 @@
         <v>185</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="14" t="s">
+    <row r="10" ht="19.5" customHeight="1" spans="1:76">
+      <c r="A10" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="15"/>
-      <c r="AM10" s="15"/>
-      <c r="AN10" s="15"/>
-      <c r="AO10" s="15"/>
-      <c r="AP10" s="15"/>
-      <c r="AQ10" s="15"/>
-      <c r="AR10" s="15"/>
-      <c r="AS10" s="15"/>
-      <c r="AT10" s="15"/>
-      <c r="AU10" s="15"/>
-      <c r="AV10" s="15"/>
-      <c r="AW10" s="15"/>
-      <c r="AX10" s="15"/>
-      <c r="AY10" s="15"/>
-      <c r="AZ10" s="15"/>
-      <c r="BA10" s="15"/>
-      <c r="BB10" s="15"/>
-      <c r="BC10" s="15"/>
-      <c r="BD10" s="15"/>
-      <c r="BE10" s="15"/>
-      <c r="BF10" s="15"/>
-      <c r="BG10" s="15"/>
-      <c r="BH10" s="15"/>
-      <c r="BI10" s="15"/>
-      <c r="BJ10" s="15"/>
-      <c r="BK10" s="15"/>
-      <c r="BL10" s="15"/>
-      <c r="BM10" s="15"/>
-      <c r="BN10" s="15"/>
-      <c r="BO10" s="15"/>
-      <c r="BP10" s="15"/>
-      <c r="BQ10" s="15"/>
-      <c r="BR10" s="15"/>
-      <c r="BS10" s="15"/>
-      <c r="BT10" s="15"/>
-      <c r="BU10" s="15"/>
-      <c r="BV10" s="15"/>
-      <c r="BW10" s="15"/>
-      <c r="BX10" s="15"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="12"/>
+      <c r="AJ10" s="12"/>
+      <c r="AK10" s="12"/>
+      <c r="AL10" s="12"/>
+      <c r="AM10" s="12"/>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="12"/>
+      <c r="AP10" s="12"/>
+      <c r="AQ10" s="12"/>
+      <c r="AR10" s="12"/>
+      <c r="AS10" s="12"/>
+      <c r="AT10" s="12"/>
+      <c r="AU10" s="12"/>
+      <c r="AV10" s="12"/>
+      <c r="AW10" s="12"/>
+      <c r="AX10" s="12"/>
+      <c r="AY10" s="12"/>
+      <c r="AZ10" s="12"/>
+      <c r="BA10" s="12"/>
+      <c r="BB10" s="12"/>
+      <c r="BC10" s="12"/>
+      <c r="BD10" s="12"/>
+      <c r="BE10" s="12"/>
+      <c r="BF10" s="12"/>
+      <c r="BG10" s="12"/>
+      <c r="BH10" s="12"/>
+      <c r="BI10" s="12"/>
+      <c r="BJ10" s="12"/>
+      <c r="BK10" s="12"/>
+      <c r="BL10" s="12"/>
+      <c r="BM10" s="12"/>
+      <c r="BN10" s="12"/>
+      <c r="BO10" s="12"/>
+      <c r="BP10" s="12"/>
+      <c r="BQ10" s="12"/>
+      <c r="BR10" s="12"/>
+      <c r="BS10" s="12"/>
+      <c r="BT10" s="12"/>
+      <c r="BU10" s="12"/>
+      <c r="BV10" s="12"/>
+      <c r="BW10" s="12"/>
+      <c r="BX10" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="41.25">
+    <row r="11" ht="41.25" customHeight="1" spans="1:76">
       <c r="A11" s="7" t="s">
         <v>232</v>
       </c>
@@ -3479,13 +4025,13 @@
       <c r="C11" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>161</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="10" t="s">
         <v>172</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -3512,7 +4058,7 @@
       <c r="N11" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="O11" s="10" t="s">
         <v>178</v>
       </c>
       <c r="P11" s="8" t="s">
@@ -3524,10 +4070,10 @@
       <c r="R11" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="S11" s="16" t="s">
+      <c r="S11" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="T11" s="10"/>
+      <c r="T11" s="18"/>
       <c r="U11" s="8" t="s">
         <v>213</v>
       </c>
@@ -3555,7 +4101,7 @@
       <c r="AC11" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="AD11" s="9" t="s">
+      <c r="AD11" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AE11" s="8" t="s">
@@ -3567,7 +4113,7 @@
       <c r="AG11" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="AH11" s="12"/>
+      <c r="AH11" s="17"/>
       <c r="AI11" s="8" t="s">
         <v>174</v>
       </c>
@@ -3586,7 +4132,7 @@
       <c r="AN11" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="AO11" s="9" t="s">
+      <c r="AO11" s="10" t="s">
         <v>178</v>
       </c>
       <c r="AP11" s="8" t="s">
@@ -3607,7 +4153,7 @@
       <c r="AU11" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="AV11" s="17" t="s">
+      <c r="AV11" s="20" t="s">
         <v>188</v>
       </c>
       <c r="AW11" s="8" t="s">
@@ -3652,7 +4198,7 @@
       <c r="BJ11" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="BK11" s="17" t="s">
+      <c r="BK11" s="20" t="s">
         <v>220</v>
       </c>
       <c r="BL11" s="8" t="s">
@@ -3695,8 +4241,8 @@
         <v>215</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="41.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" ht="41.25" customHeight="1" spans="1:76">
+      <c r="A12" s="9" t="s">
         <v>233</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -3750,20 +4296,20 @@
       <c r="R12" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="S12" s="16" t="s">
+      <c r="S12" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="T12" s="10"/>
+      <c r="T12" s="18"/>
       <c r="U12" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="V12" s="9" t="s">
+      <c r="V12" s="10" t="s">
         <v>178</v>
       </c>
       <c r="W12" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="X12" s="17" t="s">
+      <c r="X12" s="20" t="s">
         <v>220</v>
       </c>
       <c r="Y12" s="8" t="s">
@@ -3778,7 +4324,7 @@
       <c r="AB12" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="AC12" s="12"/>
+      <c r="AC12" s="17"/>
       <c r="AD12" s="8" t="s">
         <v>156</v>
       </c>
@@ -3794,7 +4340,7 @@
       <c r="AH12" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="AI12" s="9" t="s">
+      <c r="AI12" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AJ12" s="8" t="s">
@@ -3824,7 +4370,7 @@
       <c r="AR12" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="AS12" s="17" t="s">
+      <c r="AS12" s="20" t="s">
         <v>188</v>
       </c>
       <c r="AT12" s="8" t="s">
@@ -3845,7 +4391,7 @@
       <c r="AY12" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="AZ12" s="9" t="s">
+      <c r="AZ12" s="10" t="s">
         <v>172</v>
       </c>
       <c r="BA12" s="8" t="s">
@@ -3896,14 +4442,14 @@
       <c r="BP12" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="BQ12" s="9" t="s">
+      <c r="BQ12" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="BR12" s="12"/>
+      <c r="BR12" s="17"/>
       <c r="BS12" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="BT12" s="9" t="s">
+      <c r="BT12" s="10" t="s">
         <v>161</v>
       </c>
       <c r="BU12" s="8" t="s">
@@ -3919,11 +4465,11 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="41.25">
+    <row r="13" ht="41.25" customHeight="1" spans="1:76">
       <c r="A13" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>161</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -3974,8 +4520,8 @@
       <c r="R13" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="S13" s="12"/>
-      <c r="T13" s="10"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="18"/>
       <c r="U13" s="8" t="s">
         <v>176</v>
       </c>
@@ -3997,10 +4543,10 @@
       <c r="AA13" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="AB13" s="9" t="s">
+      <c r="AB13" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="AC13" s="9" t="s">
+      <c r="AC13" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AD13" s="8" t="s">
@@ -4018,7 +4564,7 @@
       <c r="AH13" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="AI13" s="17" t="s">
+      <c r="AI13" s="20" t="s">
         <v>220</v>
       </c>
       <c r="AJ13" s="8" t="s">
@@ -4081,7 +4627,7 @@
       <c r="BC13" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="BD13" s="12"/>
+      <c r="BD13" s="17"/>
       <c r="BE13" s="8" t="s">
         <v>153</v>
       </c>
@@ -4091,7 +4637,7 @@
       <c r="BG13" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="BH13" s="9" t="s">
+      <c r="BH13" s="10" t="s">
         <v>172</v>
       </c>
       <c r="BI13" s="8" t="s">
@@ -4100,7 +4646,7 @@
       <c r="BJ13" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="BK13" s="9" t="s">
+      <c r="BK13" s="10" t="s">
         <v>178</v>
       </c>
       <c r="BL13" s="8" t="s">
@@ -4127,10 +4673,10 @@
       <c r="BS13" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="BT13" s="9" t="s">
+      <c r="BT13" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="BU13" s="17" t="s">
+      <c r="BU13" s="20" t="s">
         <v>188</v>
       </c>
       <c r="BV13" s="8" t="s">
@@ -4143,8 +4689,8 @@
         <v>222</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="42">
-      <c r="A14" s="11" t="s">
+    <row r="14" ht="42" customHeight="1" spans="1:76">
+      <c r="A14" s="9" t="s">
         <v>235</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -4157,7 +4703,7 @@
       <c r="E14" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="10" t="s">
         <v>178</v>
       </c>
       <c r="G14" s="8" t="s">
@@ -4178,7 +4724,7 @@
       <c r="L14" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="M14" s="9" t="s">
+      <c r="M14" s="10" t="s">
         <v>161</v>
       </c>
       <c r="N14" s="8" t="s">
@@ -4187,17 +4733,17 @@
       <c r="O14" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="P14" s="12"/>
+      <c r="P14" s="17"/>
       <c r="Q14" s="8" t="s">
         <v>174</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="S14" s="16" t="s">
+      <c r="S14" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="T14" s="10"/>
+      <c r="T14" s="18"/>
       <c r="U14" s="8" t="s">
         <v>171</v>
       </c>
@@ -4231,17 +4777,17 @@
       <c r="AE14" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="AF14" s="12"/>
+      <c r="AF14" s="17"/>
       <c r="AG14" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="AH14" s="17" t="s">
+      <c r="AH14" s="20" t="s">
         <v>188</v>
       </c>
       <c r="AI14" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="AJ14" s="9" t="s">
+      <c r="AJ14" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AK14" s="8" t="s">
@@ -4253,7 +4799,7 @@
       <c r="AM14" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="AN14" s="12"/>
+      <c r="AN14" s="17"/>
       <c r="AO14" s="8" t="s">
         <v>179</v>
       </c>
@@ -4269,7 +4815,7 @@
       <c r="AS14" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="AT14" s="9" t="s">
+      <c r="AT14" s="10" t="s">
         <v>161</v>
       </c>
       <c r="AU14" s="8" t="s">
@@ -4278,7 +4824,7 @@
       <c r="AV14" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="AW14" s="9" t="s">
+      <c r="AW14" s="10" t="s">
         <v>178</v>
       </c>
       <c r="AX14" s="8" t="s">
@@ -4302,7 +4848,7 @@
       <c r="BD14" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="BE14" s="9" t="s">
+      <c r="BE14" s="10" t="s">
         <v>172</v>
       </c>
       <c r="BF14" s="8" t="s">
@@ -4332,7 +4878,7 @@
       <c r="BN14" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="BO14" s="17" t="s">
+      <c r="BO14" s="20" t="s">
         <v>220</v>
       </c>
       <c r="BP14" s="8" t="s">
@@ -4363,7 +4909,7 @@
         <v>189</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="42">
+    <row r="15" ht="42" customHeight="1" spans="1:76">
       <c r="A15" s="7" t="s">
         <v>236</v>
       </c>
@@ -4388,7 +4934,7 @@
       <c r="H15" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="10" t="s">
         <v>178</v>
       </c>
       <c r="J15" s="8" t="s">
@@ -4403,43 +4949,43 @@
       <c r="M15" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="N15" s="12"/>
+      <c r="N15" s="17"/>
       <c r="O15" s="8" t="s">
         <v>183</v>
       </c>
       <c r="P15" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="Q15" s="17" t="s">
+      <c r="Q15" s="20" t="s">
         <v>188</v>
       </c>
       <c r="R15" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="S15" s="16" t="s">
+      <c r="S15" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="T15" s="10"/>
+      <c r="T15" s="18"/>
       <c r="U15" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="V15" s="9" t="s">
+      <c r="V15" s="10" t="s">
         <v>161</v>
       </c>
       <c r="W15" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="X15" s="9" t="s">
+      <c r="X15" s="10" t="s">
         <v>178</v>
       </c>
       <c r="Y15" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="Z15" s="12"/>
+      <c r="Z15" s="17"/>
       <c r="AA15" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="AB15" s="17" t="s">
+      <c r="AB15" s="20" t="s">
         <v>220</v>
       </c>
       <c r="AC15" s="8" t="s">
@@ -4448,7 +4994,7 @@
       <c r="AD15" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="AE15" s="9" t="s">
+      <c r="AE15" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AF15" s="8" t="s">
@@ -4490,11 +5036,11 @@
       <c r="AR15" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="AS15" s="12"/>
+      <c r="AS15" s="17"/>
       <c r="AT15" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="AU15" s="9" t="s">
+      <c r="AU15" s="10" t="s">
         <v>172</v>
       </c>
       <c r="AV15" s="8" t="s">
@@ -4542,7 +5088,7 @@
       <c r="BJ15" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="BK15" s="9" t="s">
+      <c r="BK15" s="10" t="s">
         <v>161</v>
       </c>
       <c r="BL15" s="8" t="s">
@@ -4585,245 +5131,19 @@
         <v>196</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="18"/>
-      <c r="AG16" s="18"/>
-      <c r="AH16" s="18"/>
-      <c r="AI16" s="18"/>
-      <c r="AJ16" s="18"/>
-      <c r="AK16" s="18"/>
-      <c r="AL16" s="18"/>
-      <c r="AM16" s="18"/>
-      <c r="AN16" s="18"/>
-      <c r="AO16" s="18"/>
-      <c r="AP16" s="18"/>
-      <c r="AQ16" s="18"/>
-      <c r="AR16" s="18"/>
-      <c r="AS16" s="18"/>
-      <c r="AT16" s="18"/>
-      <c r="AU16" s="18"/>
-      <c r="AV16" s="18"/>
-      <c r="AW16" s="18"/>
-      <c r="AX16" s="18"/>
-      <c r="AY16" s="18"/>
-      <c r="AZ16" s="18"/>
-      <c r="BA16" s="18"/>
-      <c r="BB16" s="18"/>
-      <c r="BC16" s="18"/>
-      <c r="BD16" s="18"/>
-      <c r="BE16" s="18"/>
-      <c r="BF16" s="18"/>
-      <c r="BG16" s="18"/>
-      <c r="BH16" s="18"/>
-      <c r="BI16" s="18"/>
-      <c r="BJ16" s="18"/>
-      <c r="BK16" s="18"/>
-      <c r="BL16" s="18"/>
-      <c r="BM16" s="18"/>
-      <c r="BN16" s="18"/>
-      <c r="BO16" s="18"/>
-      <c r="BP16" s="18"/>
-      <c r="BQ16" s="18"/>
-      <c r="BR16" s="18"/>
-      <c r="BS16" s="18"/>
-      <c r="BT16" s="18"/>
-      <c r="BU16" s="18"/>
-      <c r="BV16" s="18"/>
-      <c r="BW16" s="18"/>
-      <c r="BX16" s="18"/>
+    <row r="16" ht="17.25" customHeight="1"/>
+    <row r="17" ht="17.25" hidden="1" customHeight="1" spans="1:1">
+      <c r="A17" s="14" t="s">
+        <v>237</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25" hidden="1">
-      <c r="A17" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="18"/>
-      <c r="Z17" s="18"/>
-      <c r="AA17" s="18"/>
-      <c r="AB17" s="18"/>
-      <c r="AC17" s="18"/>
-      <c r="AD17" s="18"/>
-      <c r="AE17" s="18"/>
-      <c r="AF17" s="18"/>
-      <c r="AG17" s="18"/>
-      <c r="AH17" s="18"/>
-      <c r="AI17" s="18"/>
-      <c r="AJ17" s="18"/>
-      <c r="AK17" s="18"/>
-      <c r="AL17" s="18"/>
-      <c r="AM17" s="18"/>
-      <c r="AN17" s="18"/>
-      <c r="AO17" s="18"/>
-      <c r="AP17" s="18"/>
-      <c r="AQ17" s="18"/>
-      <c r="AR17" s="18"/>
-      <c r="AS17" s="18"/>
-      <c r="AT17" s="18"/>
-      <c r="AU17" s="18"/>
-      <c r="AV17" s="18"/>
-      <c r="AW17" s="18"/>
-      <c r="AX17" s="18"/>
-      <c r="AY17" s="18"/>
-      <c r="AZ17" s="18"/>
-      <c r="BA17" s="18"/>
-      <c r="BB17" s="18"/>
-      <c r="BC17" s="18"/>
-      <c r="BD17" s="18"/>
-      <c r="BE17" s="18"/>
-      <c r="BF17" s="18"/>
-      <c r="BG17" s="18"/>
-      <c r="BH17" s="18"/>
-      <c r="BI17" s="18"/>
-      <c r="BJ17" s="18"/>
-      <c r="BK17" s="18"/>
-      <c r="BL17" s="18"/>
-      <c r="BM17" s="18"/>
-      <c r="BN17" s="18"/>
-      <c r="BO17" s="18"/>
-      <c r="BP17" s="18"/>
-      <c r="BQ17" s="18"/>
-      <c r="BR17" s="18"/>
-      <c r="BS17" s="18"/>
-      <c r="BT17" s="18"/>
-      <c r="BU17" s="18"/>
-      <c r="BV17" s="18"/>
-      <c r="BW17" s="18"/>
-      <c r="BX17" s="18"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25" hidden="1">
-      <c r="A18" s="20" t="s">
+    <row r="18" ht="17.25" hidden="1" customHeight="1" spans="1:1">
+      <c r="A18" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18"/>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
-      <c r="AJ18" s="18"/>
-      <c r="AK18" s="18"/>
-      <c r="AL18" s="18"/>
-      <c r="AM18" s="18"/>
-      <c r="AN18" s="18"/>
-      <c r="AO18" s="18"/>
-      <c r="AP18" s="18"/>
-      <c r="AQ18" s="18"/>
-      <c r="AR18" s="18"/>
-      <c r="AS18" s="18"/>
-      <c r="AT18" s="18"/>
-      <c r="AU18" s="18"/>
-      <c r="AV18" s="18"/>
-      <c r="AW18" s="18"/>
-      <c r="AX18" s="18"/>
-      <c r="AY18" s="18"/>
-      <c r="AZ18" s="18"/>
-      <c r="BA18" s="18"/>
-      <c r="BB18" s="18"/>
-      <c r="BC18" s="18"/>
-      <c r="BD18" s="18"/>
-      <c r="BE18" s="18"/>
-      <c r="BF18" s="18"/>
-      <c r="BG18" s="18"/>
-      <c r="BH18" s="18"/>
-      <c r="BI18" s="18"/>
-      <c r="BJ18" s="18"/>
-      <c r="BK18" s="18"/>
-      <c r="BL18" s="18"/>
-      <c r="BM18" s="18"/>
-      <c r="BN18" s="18"/>
-      <c r="BO18" s="18"/>
-      <c r="BP18" s="18"/>
-      <c r="BQ18" s="18"/>
-      <c r="BR18" s="18"/>
-      <c r="BS18" s="18"/>
-      <c r="BT18" s="18"/>
-      <c r="BU18" s="18"/>
-      <c r="BV18" s="18"/>
-      <c r="BW18" s="18"/>
-      <c r="BX18" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>